<commit_message>
uploaded some para meters in config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Jones Radiology\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navee_d\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E4C31-EA41-4FC6-9754-690969D3281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F962CC3-998D-4AAE-926C-B9A939A4035E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>Screenshots</t>
   </si>
   <si>
-    <t>RPAChallengeProcess_for_PlanIT</t>
-  </si>
-  <si>
     <t>OutputExtractedSheet</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>\Data\Output</t>
+  </si>
+  <si>
+    <t>RPA_Assignment_For_Jones_Radiology</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -642,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
@@ -1836,10 +1836,10 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -1850,7 +1850,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>